<commit_message>
updated artist list copy
</commit_message>
<xml_diff>
--- a/data/artist_list copy.xlsx
+++ b/data/artist_list copy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tylergleeson/Documents/GitHub/kpop_analytics/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B84FD86-614D-8F43-A3FC-5DA597C5C1AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BCDFBBF-6E6D-EB46-8847-89E481F2D562}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16440" xr2:uid="{6EA75BC8-7E97-A641-A26D-A554D3532DC8}"/>
   </bookViews>
@@ -39,21 +39,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>Artist</t>
   </si>
   <si>
-    <t>BOYNEXTDOOR</t>
-  </si>
-  <si>
-    <t>CHEN</t>
-  </si>
-  <si>
-    <t>CHENLE</t>
-  </si>
-  <si>
-    <t>CHO JUNYOUNG</t>
+    <t>JOHNNY CASH</t>
   </si>
 </sst>
 </file>
@@ -478,7 +469,7 @@
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A5"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -497,19 +488,13 @@
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="A3" s="2"/>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>3</v>
-      </c>
+      <c r="A4" s="2"/>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>4</v>
-      </c>
+      <c r="A5" s="2"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A53">

</xml_diff>